<commit_message>
Latest updates with new faces - 2025-04-14 12:55
</commit_message>
<xml_diff>
--- a/AttendanceData/April-2025.xlsx
+++ b/AttendanceData/April-2025.xlsx
@@ -446,12 +446,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Entry Time</t>
+          <t>EntryTime</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Exit Time</t>
+          <t>ExitTime</t>
         </is>
       </c>
     </row>
@@ -468,10 +468,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10:16:36</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>12:38:05</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update April 2025 attendance data
</commit_message>
<xml_diff>
--- a/AttendanceData/April-2025.xlsx
+++ b/AttendanceData/April-2025.xlsx
@@ -468,12 +468,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>12:38:05</t>
+          <t>15:11:52</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>12:43:32</t>
+          <t>15:12:13</t>
         </is>
       </c>
     </row>

</xml_diff>